<commit_message>
Druid, Fighter, Monk, Paladin Reorg
</commit_message>
<xml_diff>
--- a/PlaytestOptions.xlsx
+++ b/PlaytestOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7829E18D-2EE4-4B1B-B3F5-00532E4AB768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B69272-73AD-4EB2-94E1-6ED9F5B1E505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
   <si>
     <t>Class</t>
   </si>
@@ -210,9 +210,6 @@
     <t xml:space="preserve"> A primal warrior who uses a variety of battle cries to inspire allies and disrupt enemies</t>
   </si>
   <si>
-    <t>A barbarian whose rage manifests into lashing storms.  These storms can be lihting storms, sandstorms, or blizzards.</t>
-  </si>
-  <si>
     <t>A demonic warrior with highly customizable fiendish abilities that functions as a 1/3 caster</t>
   </si>
   <si>
@@ -220,6 +217,126 @@
   </si>
   <si>
     <t>An Antman-style artificer that weaves through combat by alternating between shrinking to minuscule sizes and expanding to enormous proportions</t>
+  </si>
+  <si>
+    <t>Druid</t>
+  </si>
+  <si>
+    <t>Circle of Essense</t>
+  </si>
+  <si>
+    <t>Circle of Geometry</t>
+  </si>
+  <si>
+    <t>Circle of Mountains</t>
+  </si>
+  <si>
+    <t>Circle of Restoration</t>
+  </si>
+  <si>
+    <t>Circle of Spores (Alternative)</t>
+  </si>
+  <si>
+    <t>Circle of Rivers</t>
+  </si>
+  <si>
+    <t>Circle of Grasslands</t>
+  </si>
+  <si>
+    <t>Circle of Twilight (Alternative)</t>
+  </si>
+  <si>
+    <t>Circle of Venom</t>
+  </si>
+  <si>
+    <t>Fighter</t>
+  </si>
+  <si>
+    <t>Commander</t>
+  </si>
+  <si>
+    <t>Monk</t>
+  </si>
+  <si>
+    <t>Way of the World Soul</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>Oath of Lore</t>
+  </si>
+  <si>
+    <t>A druid who manipulates the essence of life to alternate between draining vitality from enemies and restoring it to allies</t>
+  </si>
+  <si>
+    <t>A druid who summons fractal animals and creates magical geometric shapes across the battlefield to aid in combat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A high-speed druid who specializes in transforming into grasslands animals while casting high mobility spells in these forms </t>
+  </si>
+  <si>
+    <t>Front Line</t>
+  </si>
+  <si>
+    <t>Mid Line</t>
+  </si>
+  <si>
+    <t>Back Line</t>
+  </si>
+  <si>
+    <t>A druid who specializes in transforming into mountain-dwelling animals, casting mountain themed spells, and even summoning miniature mountains</t>
+  </si>
+  <si>
+    <t>A druid who specializes in healing and enhancing multiple allies while simultaneously attacking enemies</t>
+  </si>
+  <si>
+    <t>A druid who specializes in transforming into river animals, casting river-themed spells, and even summoning miniature rivers</t>
+  </si>
+  <si>
+    <t>A fungus themed druid who fights using deadly spores and grows fungal minions from the corpses of enemies</t>
+  </si>
+  <si>
+    <t>A scythe-wielding druid who reaps foes and manipulates the line between life and death</t>
+  </si>
+  <si>
+    <t>A poison themed druid who specializes in transforming into venomous creatures</t>
+  </si>
+  <si>
+    <t>A selfless fighter who organizes the party and lends a helping hand to teammates in need</t>
+  </si>
+  <si>
+    <t>A monk who shares ki and martial arts abilities with allies through soul bonds</t>
+  </si>
+  <si>
+    <t>A versatile adventuring historian with access to advanced combat maneuvers, a wide range of skills, and aid from ancient spirits</t>
+  </si>
+  <si>
+    <t>Broken Oath - Madness</t>
+  </si>
+  <si>
+    <t>An oathbreaker who uses terror and illusions to isolate and control victims</t>
+  </si>
+  <si>
+    <t>Oath of The Legion</t>
+  </si>
+  <si>
+    <t>Oath of Vengeance (Alternative)</t>
+  </si>
+  <si>
+    <t>Oath of Wrath</t>
+  </si>
+  <si>
+    <t>A barbarian whose rage manifests into lashing storms.  These storms can be lightning storms, sandstorms, or blizzards.</t>
+  </si>
+  <si>
+    <t>An inspiring paladin who wields and casts spells through a weaponized, enchanted, throwable banner</t>
+  </si>
+  <si>
+    <t>An aggressive paladin that mercilessly hunts down chosen foes in battle</t>
+  </si>
+  <si>
+    <t>A flame wielding paladin that ruthlessly burns down evil doers en masse</t>
   </si>
 </sst>
 </file>
@@ -301,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,6 +456,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -350,6 +473,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -632,170 +761,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC14"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="3"/>
-    <col min="13" max="13" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="4"/>
-    <col min="16" max="16" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="9.140625" style="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="4"/>
+    <col min="18" max="18" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="9.140625" style="1"/>
+    <col min="31" max="31" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:31" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="12" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="16" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="AA1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-    </row>
-    <row r="2" spans="1:29" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="8" t="s">
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+    </row>
+    <row r="2" spans="1:31" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="Y2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="7" t="s">
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AB2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AD2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AE2" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -803,13 +944,15 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -817,13 +960,13 @@
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -831,13 +974,13 @@
         <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -845,13 +988,13 @@
         <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -865,7 +1008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -879,7 +1022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -893,7 +1036,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -907,7 +1050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -921,7 +1064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -935,7 +1078,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -949,7 +1092,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
@@ -963,17 +1106,241 @@
         <v>37</v>
       </c>
     </row>
+    <row r="15" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="Y1:AC1"/>
-    <mergeCell ref="F1:O1"/>
-    <mergeCell ref="P1:W1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="H1:Q1"/>
+    <mergeCell ref="R1:Y1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{93495F71-B436-49A2-8013-B6E6FCD1C889}"/>
@@ -988,8 +1355,24 @@
     <hyperlink ref="B12" r:id="rId10" xr:uid="{B18ED3DA-E6DA-4B85-9688-B63504775A85}"/>
     <hyperlink ref="B13" r:id="rId11" xr:uid="{11172451-FD87-4C25-8DFC-2B12F8D7CD9B}"/>
     <hyperlink ref="B14" r:id="rId12" xr:uid="{67502A12-BA18-4C6E-ADF2-1CB1FB7E44AE}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{CDA22DD6-58D7-4CD3-A5B1-7664D9A10B17}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{D3322A7D-5320-4B8D-BCB3-0B064925BC7B}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{634A2B13-8B8A-474E-903A-48756F0390BC}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{5FC76316-029E-4C93-91EB-EC292F079013}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{EEA47A3E-3619-439C-A62E-A20F471EC74B}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{93568C5D-95D9-4F2B-B917-65DEA5E91E23}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{EE816124-5CB0-4A4F-9E7E-5A0092AFD7EF}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{73BCB1B2-F6A9-4843-8B73-266CE9845469}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{68D42396-F42B-4C72-9061-039919CD847C}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{A0F8F097-546B-4331-858C-14FCA4FF7026}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{EAA64930-197B-4768-AA8E-0C289CA89CE0}"/>
+    <hyperlink ref="B27" r:id="rId24" xr:uid="{31E306F5-6F8A-4CB2-8762-BFD75ED9C89C}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{B8232798-2786-4E9E-B5A5-EDAA516CA38B}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{782F7782-5B75-4475-8662-2240197F24FF}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{081C73CA-EB26-40FB-80EA-64B7BE0AA480}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{C6DD030D-9F8C-4272-929A-0EACEC073E5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ReOrg for Remainder of Suclasses
</commit_message>
<xml_diff>
--- a/PlaytestOptions.xlsx
+++ b/PlaytestOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7460D9-FE13-41C0-A559-CDB8118A7386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CFDE48-D9EA-4B74-851E-D7DBBA6C55CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="133">
   <si>
     <t>Class</t>
   </si>
@@ -358,6 +358,72 @@
   </si>
   <si>
     <t>A whaler-inspired ranger always looking for the next big catch who fights using nets and harpoons</t>
+  </si>
+  <si>
+    <t>Rogue</t>
+  </si>
+  <si>
+    <t>Deadeye</t>
+  </si>
+  <si>
+    <t>Spellthief</t>
+  </si>
+  <si>
+    <t>A sharpshooting rogue who fires carefully aimed trick shots capable of inflicting a variety of effects upon their targets</t>
+  </si>
+  <si>
+    <t>A rogue who uses sneak attacks to steal spells and other supernatural abilities from targets</t>
+  </si>
+  <si>
+    <t>Sorcerer</t>
+  </si>
+  <si>
+    <t>Elemental Conflux</t>
+  </si>
+  <si>
+    <t>A sorcerer who wields and combines the elemental powers of earth, fire, water, and wind into customized elemental spells and summoned elemental amalgams</t>
+  </si>
+  <si>
+    <t>Wild Magic (Alternative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A chaotic caster who can unleash powerful spells at random and whose magic occasionally causes unpredictable arcane anomalies </t>
+  </si>
+  <si>
+    <t>Warlock</t>
+  </si>
+  <si>
+    <t>Otherworldly Patron - The Council</t>
+  </si>
+  <si>
+    <t>Otherworldly Patron - The Influencer</t>
+  </si>
+  <si>
+    <t>Otherworlderly Patron - The Cauldron</t>
+  </si>
+  <si>
+    <t>An apothecary who draws eldritch power from an enchanted cauldron and harvests ingredients to brew into arcane concoctions</t>
+  </si>
+  <si>
+    <t>A warlock who's made a pact with some form of mystical organization and is capable of creating and enforcing magical contracts to control others</t>
+  </si>
+  <si>
+    <t>A brazen warlock who's made a pact to achieve fame or influence over others and can use these powers to belittle and diminish the abilities of enemies</t>
+  </si>
+  <si>
+    <t>Wizard</t>
+  </si>
+  <si>
+    <t>School of Invention (Alternate)</t>
+  </si>
+  <si>
+    <t>School of Numerology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A reckless innovator who uses an arcane apparatus to enhance spells, pushing its power to the limit at the risk of magical disaster </t>
+  </si>
+  <si>
+    <t>A mathemagician who uses magic numbers to solve arcane equations which can be used to alter the nature of reality in calculated ways</t>
   </si>
 </sst>
 </file>
@@ -782,17 +848,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE33"/>
+  <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -1391,6 +1457,132 @@
       </c>
       <c r="D33" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1437,8 +1629,17 @@
     <hyperlink ref="B31" r:id="rId29" xr:uid="{3AF3F6EE-CE6F-455C-A0EB-A5C61287B5CA}"/>
     <hyperlink ref="B32" r:id="rId30" xr:uid="{F2B8D2B5-D925-43E8-BDCD-BC849E66F893}"/>
     <hyperlink ref="B33" r:id="rId31" xr:uid="{B71AE17B-4FBF-481D-BDA6-09CFBE3EBCF4}"/>
+    <hyperlink ref="B34" r:id="rId32" xr:uid="{EB1F7152-3946-42A1-B78E-9CDA78D08240}"/>
+    <hyperlink ref="B35" r:id="rId33" xr:uid="{4F24CD04-9548-48F6-96BB-A2A221528C48}"/>
+    <hyperlink ref="B36" r:id="rId34" xr:uid="{8ADB10D1-DE45-4B43-B4CC-FC4A2547D8E8}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{108963DA-E279-49AA-8696-0AEABB87D523}"/>
+    <hyperlink ref="B38" r:id="rId36" xr:uid="{2267B16F-FD78-47AA-A448-4E3F18595A84}"/>
+    <hyperlink ref="B39" r:id="rId37" xr:uid="{B02E6E63-A75E-439E-A409-4E9A268DA50A}"/>
+    <hyperlink ref="B40" r:id="rId38" xr:uid="{BCED63E1-55A4-4F42-82FE-2952B582019E}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{1C99A195-A3F2-4110-BAC4-0B33B4EC29F5}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{FEB228C6-716E-4818-B0CB-D9908B1B5289}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId32"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>